<commit_message>
clean up of transcripts for referential, matching ids
</commit_message>
<xml_diff>
--- a/data/expt_2/raw_transcripts/game24.xlsx
+++ b/data/expt_2/raw_transcripts/game24.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="171">
   <si>
     <t xml:space="preserve">start</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
+    <t xml:space="preserve">on_topic</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Okay, now you're on camera.</t>
   </si>
   <si>
@@ -200,6 +203,9 @@
   </si>
   <si>
     <t xml:space="preserve">An apple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
   </si>
   <si>
     <t xml:space="preserve">Okay, [id71] and you press what you think is in the black box.</t>
@@ -609,7 +615,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -619,6 +625,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -745,12 +755,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H170"/>
+  <dimension ref="A1:I170"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H166" activeCellId="0" sqref="H166"/>
+      <selection pane="bottomLeft" activeCell="I165" activeCellId="0" sqref="I165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -758,8 +768,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="56.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="2.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,6 +798,9 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -796,10 +810,10 @@
         <v>1600</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,10 +824,10 @@
         <v>4140</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,10 +838,10 @@
         <v>8000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,10 +852,10 @@
         <v>9760</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -852,10 +866,10 @@
         <v>12260</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,10 +880,10 @@
         <v>14220</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,10 +894,10 @@
         <v>20940</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,10 +908,10 @@
         <v>24940</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -908,10 +922,10 @@
         <v>29240</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,10 +936,10 @@
         <v>30860</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,10 +950,10 @@
         <v>32620</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,10 +964,10 @@
         <v>33320</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,10 +978,10 @@
         <v>34920</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,10 +992,10 @@
         <v>39640</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,10 +1006,10 @@
         <v>40160</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,10 +1020,10 @@
         <v>41380</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1020,10 +1034,10 @@
         <v>43340</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1034,10 +1048,10 @@
         <v>44980</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1048,10 +1062,10 @@
         <v>45320</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,10 +1076,10 @@
         <v>45840</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,10 +1090,10 @@
         <v>47780</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,10 +1104,10 @@
         <v>48820</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,10 +1118,10 @@
         <v>49820</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,10 +1132,10 @@
         <v>54820</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,10 +1146,10 @@
         <v>59820</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1146,10 +1160,10 @@
         <v>61820</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,10 +1174,10 @@
         <v>65820</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,10 +1188,10 @@
         <v>73820</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,10 +1202,10 @@
         <v>77820</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,10 +1216,10 @@
         <v>81580</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1216,10 +1230,10 @@
         <v>87720</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,10 +1244,10 @@
         <v>92580</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,10 +1258,10 @@
         <v>95460</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1258,10 +1272,10 @@
         <v>100380</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,10 +1286,10 @@
         <v>105820</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,10 +1300,10 @@
         <v>105820</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,10 +1314,10 @@
         <v>105820</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,10 +1328,10 @@
         <v>105820</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,10 +1342,10 @@
         <v>107940</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,10 +1356,10 @@
         <v>110540</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,10 +1370,10 @@
         <v>115180</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,10 +1384,10 @@
         <v>117240</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,10 +1398,10 @@
         <v>120820</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,10 +1412,10 @@
         <v>122360</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1412,10 +1426,10 @@
         <v>127300</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1426,10 +1440,10 @@
         <v>131980</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,10 +1454,10 @@
         <v>133700</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E48" s="2" t="n">
         <v>0</v>
@@ -1457,13 +1471,13 @@
         <v>141200</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,10 +1488,10 @@
         <v>141200</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1488,16 +1502,19 @@
         <v>147040</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,10 +1525,10 @@
         <v>147040</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,10 +1539,10 @@
         <v>163680</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1536,10 +1553,10 @@
         <v>163680</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E54" s="2" t="n">
         <v>1</v>
@@ -1553,10 +1570,10 @@
         <v>170400</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,16 +1584,19 @@
         <v>170400</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,13 +1607,16 @@
         <v>170400</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,10 +1627,10 @@
         <v>170400</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,10 +1641,10 @@
         <v>180480</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E59" s="2" t="n">
         <v>2</v>
@@ -1635,16 +1658,19 @@
         <v>188400</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1655,10 +1681,10 @@
         <v>188400</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1669,10 +1695,10 @@
         <v>193200</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1683,13 +1709,16 @@
         <v>193200</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1700,10 +1729,10 @@
         <v>193200</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,10 +1743,10 @@
         <v>199440</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E65" s="2" t="n">
         <v>3</v>
@@ -1731,16 +1760,19 @@
         <v>199440</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1751,10 +1783,10 @@
         <v>205600</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1765,13 +1797,16 @@
         <v>206400</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,10 +1817,10 @@
         <v>210960</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E69" s="2" t="n">
         <v>4</v>
@@ -1799,16 +1834,19 @@
         <v>216960</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,10 +1857,10 @@
         <v>223040</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1833,15 +1871,18 @@
         <v>225040</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H72" s="2"/>
+      <c r="I72" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
@@ -1851,10 +1892,10 @@
         <v>232040</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,13 +1906,16 @@
         <v>234040</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1882,10 +1926,10 @@
         <v>238040</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G75" s="2"/>
     </row>
@@ -1897,10 +1941,10 @@
         <v>241040</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1911,16 +1955,19 @@
         <v>252040</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1931,10 +1978,10 @@
         <v>255040</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,16 +1992,19 @@
         <v>257040</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1965,13 +2015,16 @@
         <v>260040</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,10 +2035,10 @@
         <v>262040</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E81" s="2"/>
     </row>
@@ -1997,10 +2050,10 @@
         <v>264040</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E82" s="2" t="n">
         <v>5</v>
@@ -2014,10 +2067,10 @@
         <v>265040</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,10 +2081,10 @@
         <v>269040</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,10 +2095,10 @@
         <v>272040</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2056,10 +2109,10 @@
         <v>274040</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,16 +2123,19 @@
         <v>274040</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,13 +2146,13 @@
         <v>275040</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2107,10 +2163,10 @@
         <v>288040</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2121,10 +2177,10 @@
         <v>289040</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E90" s="2"/>
     </row>
@@ -2136,10 +2192,10 @@
         <v>291040</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E91" s="2" t="n">
         <v>6</v>
@@ -2153,10 +2209,10 @@
         <v>295040</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2167,16 +2223,19 @@
         <v>300040</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2187,13 +2246,16 @@
         <v>300040</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2204,10 +2266,10 @@
         <v>302040</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,10 +2280,10 @@
         <v>308040</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E96" s="2" t="n">
         <v>7</v>
@@ -2235,10 +2297,10 @@
         <v>309040</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2249,10 +2311,10 @@
         <v>312040</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2263,16 +2325,19 @@
         <v>315040</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2283,10 +2348,10 @@
         <v>316040</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,10 +2362,10 @@
         <v>318040</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E101" s="2" t="n">
         <v>8</v>
@@ -2314,10 +2379,10 @@
         <v>324040</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2328,10 +2393,10 @@
         <v>329040</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2342,16 +2407,19 @@
         <v>330040</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,10 +2430,10 @@
         <v>332040</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,10 +2444,10 @@
         <v>333040</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E106" s="2" t="n">
         <v>9</v>
@@ -2393,10 +2461,10 @@
         <v>334040</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,10 +2475,10 @@
         <v>336040</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,16 +2489,19 @@
         <v>338040</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="I109" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2441,13 +2512,16 @@
         <v>357040</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2458,10 +2532,10 @@
         <v>359040</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2472,10 +2546,10 @@
         <v>361040</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E112" s="2" t="n">
         <v>10</v>
@@ -2489,10 +2563,10 @@
         <v>364040</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2503,10 +2577,10 @@
         <v>369040</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2517,16 +2591,19 @@
         <v>371040</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2537,13 +2614,13 @@
         <v>374040</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2554,10 +2631,10 @@
         <v>378040</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E117" s="2" t="n">
         <v>11</v>
@@ -2571,10 +2648,10 @@
         <v>382040</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2585,10 +2662,10 @@
         <v>391040</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2599,13 +2676,16 @@
         <v>394040</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,10 +2696,10 @@
         <v>396040</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2630,16 +2710,19 @@
         <v>398040</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2650,10 +2733,10 @@
         <v>400040</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,10 +2747,10 @@
         <v>402040</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E124" s="2" t="n">
         <v>12</v>
@@ -2681,10 +2764,10 @@
         <v>404040</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2695,10 +2778,10 @@
         <v>407040</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F126" s="2"/>
     </row>
@@ -2710,16 +2793,19 @@
         <v>410040</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2730,13 +2816,13 @@
         <v>411040</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2747,10 +2833,10 @@
         <v>428000</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2761,10 +2847,10 @@
         <v>428000</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E130" s="2" t="n">
         <v>13</v>
@@ -2778,16 +2864,19 @@
         <v>428000</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="I131" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,10 +2887,10 @@
         <v>430000</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E132" s="2" t="n">
         <v>14</v>
@@ -2815,10 +2904,10 @@
         <v>436000</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2829,16 +2918,19 @@
         <v>442000</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2849,13 +2941,16 @@
         <v>446000</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2866,16 +2961,19 @@
         <v>450000</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2886,13 +2984,16 @@
         <v>450000</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2903,10 +3004,10 @@
         <v>452000</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E138" s="2" t="n">
         <v>15</v>
@@ -2920,10 +3021,10 @@
         <v>457000</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2934,16 +3035,19 @@
         <v>464000</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H140" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2954,10 +3058,10 @@
         <v>468000</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E141" s="2" t="n">
         <v>16</v>
@@ -2971,10 +3075,10 @@
         <v>472000</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2985,16 +3089,19 @@
         <v>475000</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="I143" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3005,13 +3112,16 @@
         <v>475000</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3022,10 +3132,10 @@
         <v>478000</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E145" s="2" t="n">
         <v>17</v>
@@ -3039,10 +3149,10 @@
         <v>484000</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3053,16 +3163,19 @@
         <v>491000</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3073,10 +3186,10 @@
         <v>494000</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E148" s="2" t="n">
         <v>18</v>
@@ -3090,10 +3203,10 @@
         <v>505000</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3104,13 +3217,16 @@
         <v>512000</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3121,10 +3237,10 @@
         <v>515000</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3135,13 +3251,16 @@
         <v>517000</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3152,10 +3271,10 @@
         <v>519000</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3166,16 +3285,19 @@
         <v>521000</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H154" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,13 +3308,16 @@
         <v>524000</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3203,10 +3328,10 @@
         <v>527000</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3217,10 +3342,10 @@
         <v>529000</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E157" s="2" t="n">
         <v>19</v>
@@ -3234,13 +3359,13 @@
         <v>530000</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3251,10 +3376,10 @@
         <v>532000</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3265,10 +3390,10 @@
         <v>535000</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3279,13 +3404,13 @@
         <v>535000</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3296,10 +3421,10 @@
         <v>536000</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3310,10 +3435,10 @@
         <v>539000</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3324,16 +3449,19 @@
         <v>540000</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H164" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
+      </c>
+      <c r="I164" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3344,10 +3472,10 @@
         <v>542000</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3358,10 +3486,10 @@
         <v>543000</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,10 +3500,10 @@
         <v>549000</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3386,10 +3514,10 @@
         <v>552000</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3400,10 +3528,10 @@
         <v>554000</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3414,10 +3542,10 @@
         <v>556000</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>